<commit_message>
[FIX] plan_revision and fix bug
</commit_message>
<xml_diff>
--- a/budget_plan_excel/templates/budget_plan.xlsx
+++ b/budget_plan_excel/templates/budget_plan.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Released Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount</t>
+    <t xml:space="preserve">New Amount</t>
   </si>
   <si>
     <t xml:space="preserve">Consumed</t>
@@ -289,7 +289,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>